<commit_message>
Updated Master.xls to include fasteners per-tray including unchecked items. Highlighted Fasteners/Bill of Materials - Fasteners.xlsx with questions regarding what goes where - Tnguyen
git-svn-id: svn+ssh://localhost/home/pcb/svn@589 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/Bill of Materials masterlist/External/Fasteners/Bill of Materials - Fasteners.xlsx
+++ b/Bill of Materials masterlist/External/Fasteners/Bill of Materials - Fasteners.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="600" windowWidth="27315" windowHeight="12780"/>
+    <workbookView xWindow="-900" yWindow="330" windowWidth="27315" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -121,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,13 +137,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -167,12 +191,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +505,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,146 +565,146 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <f>B4+C4+D4+E4+F4+G4</f>
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <f>H4-I4</f>
         <v>2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="5">
         <v>77.61</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>8</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>16</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <f t="shared" ref="H5:H7" si="0">B5+C5+D5+E5+F5+G5</f>
         <v>32</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>16</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <f t="shared" ref="J5:J7" si="1">H5-I5</f>
         <v>16</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="8">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="4">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>33</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>8</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>33</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="6">
         <v>74</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>14</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <v>14</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <f t="shared" ref="H8:H13" si="2">B8+C8+D8+E8+F8+G8</f>
         <v>28</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <f t="shared" ref="J8:J13" si="3">H8-I8</f>
         <v>28</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -684,7 +712,7 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>2</v>
       </c>
       <c r="H9">
@@ -709,7 +737,7 @@
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>2</v>
       </c>
       <c r="H10">
@@ -759,7 +787,7 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>8</v>
       </c>
       <c r="E12">
@@ -787,10 +815,10 @@
       <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>16</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>16</v>
       </c>
       <c r="H13">
@@ -818,6 +846,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>